<commit_message>
Add 7 and 8 results
</commit_message>
<xml_diff>
--- a/pa2/results.xlsx
+++ b/pa2/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradwest/drive/msu/spring2019/csci566/csci566_pa/pa2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{15ECFF64-C21E-8747-B905-0EFFB86E6BB4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{429A3260-33ED-8F46-B191-C38E64EAD8AB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="460" windowWidth="25240" windowHeight="15700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="460" windowWidth="25240" windowHeight="15700" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exp_1" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -3473,8 +3473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3524,6 +3524,15 @@
       <c r="F2">
         <v>32</v>
       </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
@@ -3542,6 +3551,15 @@
       <c r="F3">
         <v>32</v>
       </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
@@ -3560,6 +3578,15 @@
       <c r="F4">
         <v>32</v>
       </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
@@ -3578,6 +3605,15 @@
       <c r="F5">
         <v>32</v>
       </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1.1764705882352899</v>
+      </c>
+      <c r="I5">
+        <v>1.9607843137254899</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
@@ -3596,6 +3632,15 @@
       <c r="F6">
         <v>32</v>
       </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1.2</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
@@ -3614,6 +3659,15 @@
       <c r="F7">
         <v>32</v>
       </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1.19215686274509</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
@@ -3632,6 +3686,15 @@
       <c r="F8">
         <v>32</v>
       </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>3.73700088731144</v>
+      </c>
+      <c r="I8">
+        <v>6.5217391304347698</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
@@ -3650,6 +3713,15 @@
       <c r="F9">
         <v>32</v>
       </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
@@ -3668,6 +3740,15 @@
       <c r="F10">
         <v>32</v>
       </c>
+      <c r="G10">
+        <v>1.9607843137254899</v>
+      </c>
+      <c r="H10">
+        <v>1.9921568627451001</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
@@ -3686,6 +3767,15 @@
       <c r="F11">
         <v>32</v>
       </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0.81632653061224503</v>
+      </c>
+      <c r="I11">
+        <v>4.0816326530612201</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
@@ -3704,6 +3794,15 @@
       <c r="F12">
         <v>32</v>
       </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1.60032012805122</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
@@ -3720,6 +3819,15 @@
       </c>
       <c r="F13">
         <v>32</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -3739,6 +3847,15 @@
       <c r="F14">
         <v>32</v>
       </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0.39215686274509798</v>
+      </c>
+      <c r="I14">
+        <v>1.9607843137254899</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
@@ -3757,6 +3874,15 @@
       <c r="F15">
         <v>32</v>
       </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0.39215686274509798</v>
+      </c>
+      <c r="I15">
+        <v>1.9607843137254899</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
@@ -3775,8 +3901,17 @@
       <c r="F16">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1.97647058823529</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -3793,8 +3928,17 @@
       <c r="F17">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1.9921568627451001</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -3811,8 +3955,17 @@
       <c r="F18">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1.19215686274509</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>11</v>
       </c>
@@ -3829,8 +3982,17 @@
       <c r="F19">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>5.8576752440106397</v>
+      </c>
+      <c r="I19">
+        <v>13.043478260869501</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>11</v>
       </c>
@@ -3847,8 +4009,17 @@
       <c r="F20">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1.5610859728506801</v>
+      </c>
+      <c r="I20">
+        <v>1.9607843137254899</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>11</v>
       </c>
@@ -3865,8 +4036,17 @@
       <c r="F21">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>1.9607843137254899</v>
+      </c>
+      <c r="H21">
+        <v>3.5921568627450999</v>
+      </c>
+      <c r="I21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>11</v>
       </c>
@@ -3883,8 +4063,17 @@
       <c r="F22">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>1.9607843137254899</v>
+      </c>
+      <c r="H22">
+        <v>3.6088035214085599</v>
+      </c>
+      <c r="I22">
+        <v>6.1224489795918302</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>11</v>
       </c>
@@ -3900,6 +4089,15 @@
       </c>
       <c r="F23">
         <v>32</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>2.80880352140856</v>
+      </c>
+      <c r="I23">
+        <v>6.1224489795918302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add question 9 results
</commit_message>
<xml_diff>
--- a/pa2/results.xlsx
+++ b/pa2/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradwest/drive/msu/spring2019/csci566/csci566_pa/pa2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5744674C-899B-D24B-ABFE-D4F1FBA4B719}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AB130871-7FF5-B544-A729-2DCC4E715290}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="460" windowWidth="25240" windowHeight="15700" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="460" windowWidth="25240" windowHeight="15700" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exp_1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="27">
   <si>
     <t>UDP</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>*UDP is connection-less</t>
+  </si>
+  <si>
+    <t>* begin fragmentation</t>
+  </si>
+  <si>
+    <t>na</t>
   </si>
 </sst>
 </file>
@@ -4175,7 +4181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -4582,15 +4588,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -4613,7 +4619,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -4629,8 +4635,11 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -4647,8 +4656,11 @@
         <f>F2*2</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -4665,8 +4677,11 @@
         <f t="shared" ref="F4:F22" si="0">F3*2</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -4683,8 +4698,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -4701,8 +4719,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -4719,8 +4740,11 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -4737,8 +4761,11 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -4755,8 +4782,11 @@
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -4773,8 +4803,11 @@
         <f t="shared" si="0"/>
         <v>256</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -4791,8 +4824,11 @@
         <f t="shared" si="0"/>
         <v>512</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -4809,8 +4845,11 @@
         <f t="shared" si="0"/>
         <v>1024</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -4827,8 +4866,14 @@
         <f t="shared" si="0"/>
         <v>2048</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>48</v>
+      </c>
+      <c r="H13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -4845,8 +4890,11 @@
         <f t="shared" si="0"/>
         <v>4096</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -4863,8 +4911,11 @@
         <f t="shared" si="0"/>
         <v>8192</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -4881,8 +4932,11 @@
         <f t="shared" si="0"/>
         <v>16384</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -4899,8 +4953,11 @@
         <f t="shared" si="0"/>
         <v>32768</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>10</v>
       </c>
@@ -4917,8 +4974,11 @@
         <f t="shared" si="0"/>
         <v>65536</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>10</v>
       </c>
@@ -4935,8 +4995,11 @@
         <f t="shared" si="0"/>
         <v>131072</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>10</v>
       </c>
@@ -4953,8 +5016,11 @@
         <f t="shared" si="0"/>
         <v>262144</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>10</v>
       </c>
@@ -4971,8 +5037,11 @@
         <f t="shared" si="0"/>
         <v>524288</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>10</v>
       </c>
@@ -4988,6 +5057,9 @@
       <c r="F22">
         <f t="shared" si="0"/>
         <v>1048576</v>
+      </c>
+      <c r="G22" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add larger byte values
</commit_message>
<xml_diff>
--- a/pa2/results.xlsx
+++ b/pa2/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradwest/drive/msu/spring2019/csci566/csci566_pa/pa2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AB130871-7FF5-B544-A729-2DCC4E715290}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{303C2624-E4CE-C443-B067-87808732CA2B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="460" windowWidth="25240" windowHeight="15700" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="27">
   <si>
     <t>UDP</t>
   </si>
@@ -4591,7 +4591,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4953,8 +4953,8 @@
         <f t="shared" si="0"/>
         <v>32768</v>
       </c>
-      <c r="G17" t="s">
-        <v>26</v>
+      <c r="G17">
+        <v>468</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add analysis, q10 shell script, updates to client for q 10
</commit_message>
<xml_diff>
--- a/pa2/results.xlsx
+++ b/pa2/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradwest/drive/msu/spring2019/csci566/csci566_pa/pa2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{303C2624-E4CE-C443-B067-87808732CA2B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{16C9A677-B54A-374F-8A46-85A1E0B33DC9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="460" windowWidth="25240" windowHeight="15700" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="460" windowWidth="25240" windowHeight="15700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="exp_1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="27">
   <si>
     <t>UDP</t>
   </si>
@@ -434,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -502,7 +502,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -540,6 +540,9 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -558,8 +561,20 @@
       <c r="G2">
         <v>256</v>
       </c>
+      <c r="H2">
+        <v>3.0956029891967701E-2</v>
+      </c>
+      <c r="I2">
+        <v>3.1160253744858899E-2</v>
+      </c>
+      <c r="J2">
+        <v>3.2351970672607401E-2</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -579,8 +594,20 @@
         <f>G2/2</f>
         <v>128</v>
       </c>
+      <c r="H3">
+        <v>3.0949592590332E-2</v>
+      </c>
+      <c r="I3">
+        <v>3.1083524227142299E-2</v>
+      </c>
+      <c r="J3">
+        <v>3.1283617019653299E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -600,8 +627,20 @@
         <f t="shared" ref="G4:G10" si="0">G3/2</f>
         <v>64</v>
       </c>
+      <c r="H4">
+        <v>3.0978918075561499E-2</v>
+      </c>
+      <c r="I4">
+        <v>3.1113496193519E-2</v>
+      </c>
+      <c r="J4">
+        <v>3.1389951705932603E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -621,8 +660,20 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
+      <c r="H5">
+        <v>3.08954715728759E-2</v>
+      </c>
+      <c r="I5">
+        <v>3.1074872383704499E-2</v>
+      </c>
+      <c r="J5">
+        <v>3.1439781188964802E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -642,8 +693,20 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
+      <c r="H6">
+        <v>3.0788183212280201E-2</v>
+      </c>
+      <c r="I6">
+        <v>3.0977189540862999E-2</v>
+      </c>
+      <c r="J6">
+        <v>3.1207561492919901E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -663,8 +726,20 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="H7">
+        <v>3.0765533447265601E-2</v>
+      </c>
+      <c r="I7">
+        <v>3.0928405431600699E-2</v>
+      </c>
+      <c r="J7">
+        <v>3.1269073486328097E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -684,8 +759,20 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="H8">
+        <v>3.0736684799194301E-2</v>
+      </c>
+      <c r="I8">
+        <v>3.0900579232435901E-2</v>
+      </c>
+      <c r="J8">
+        <v>3.1119823455810498E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -705,8 +792,20 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="H9">
+        <v>3.0732154846191399E-2</v>
+      </c>
+      <c r="I9">
+        <v>3.0891730235173099E-2</v>
+      </c>
+      <c r="J9">
+        <v>3.1092405319213801E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -725,6 +824,15 @@
       <c r="G10">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+      <c r="H10">
+        <v>3.0709505081176699E-2</v>
+      </c>
+      <c r="I10">
+        <v>3.08484205832848E-2</v>
+      </c>
+      <c r="J10">
+        <v>3.1126022338867101E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3480,7 +3588,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4590,7 +4698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>

</xml_diff>